<commit_message>
generates random code and adds to database
</commit_message>
<xml_diff>
--- a/database_offline.xlsx
+++ b/database_offline.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4272" yWindow="588" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="accountInfo" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="store" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -395,7 +395,7 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -444,7 +444,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>The Witcher 3: Wild Hunt/Civilization VI/Half-Life: Alyx/Command &amp; Conquer/Doom</t>
+          <t>The Witcher 3: Wild Hunt/Civilization VI/Half-Life: Alyx/Command &amp; Conquer/Doom/Stardew Valley/Portal/RollerCoaster Tycoon/Team Fortress 2/The Sims/RollerCoaster Tycoon 2</t>
         </is>
       </c>
       <c r="E2" s="2" t="n"/>
@@ -467,7 +467,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Doom/Stardew Valley/Minecraft/Civilization VI</t>
+          <t>Doom/Stardew Valley/Minecraft/Civilization VI/The Witcher 3: Wild Hunt/Celeste</t>
         </is>
       </c>
       <c r="E3" s="2" t="n"/>
@@ -505,6 +505,11 @@
           <t>rachel5@gmail.com</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Civilization VI/The Witcher 3: Wild Hunt/Celeste/Doom/Stardew Valley/Cuphead/Portal</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -539,6 +544,11 @@
           <t>jose12@gmail.com</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Age of Empires/Doom/The Witcher 3: Wild Hunt/Portal/Celeste/Half-Life: Alyx/Stardew Valley/Myst/Tetris Effect/RollerCoaster Tycoon/The Sims/Minecraft</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -624,7 +634,11 @@
           <t>jo99@gmail.com</t>
         </is>
       </c>
-      <c r="D12" s="3" t="n"/>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>Fallout/The Witcher 3: Wild Hunt/The Sims</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
@@ -672,10 +686,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -711,6 +725,11 @@
           <t>Release_Date</t>
         </is>
       </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Valid_Codes</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="5" t="n"/>
@@ -759,6 +778,11 @@
       <c r="F3" s="9" t="n">
         <v>2016</v>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>087QB0A/OJBNA1W</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="5" t="n"/>
@@ -783,6 +807,11 @@
       <c r="F4" s="9" t="n">
         <v>2020</v>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>D2WKY6W</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" s="5" t="n"/>
@@ -807,6 +836,11 @@
       <c r="F5" s="9" t="n">
         <v>2018</v>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>AVDF58I/PFCG169</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" s="5" t="n"/>
@@ -854,6 +888,11 @@
       </c>
       <c r="F7" s="9" t="n">
         <v>1993</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Y6BAP56</t>
+        </is>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Added functional recent games area
</commit_message>
<xml_diff>
--- a/database_offline.xlsx
+++ b/database_offline.xlsx
@@ -399,7 +399,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="21.21875" customWidth="1" min="3" max="3"/>
   </cols>
@@ -422,7 +422,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Library</t>
+          <t>Library/Civilization VI</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
more codes for unit testing
</commit_message>
<xml_diff>
--- a/database_offline.xlsx
+++ b/database_offline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38340" yWindow="3045" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="accountInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -409,12 +409,12 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col width="21.28515625" customWidth="1" min="3" max="3"/>
+    <col width="21.33203125" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -457,7 +457,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>The Witcher 3: Wild Hunt/Civilization VI/Half-Life: Alyx/Command &amp; Conquer/Doom/Stardew Valley/Portal/RollerCoaster Tycoon/Team Fortress 2/The Sims/RollerCoaster Tycoon 2</t>
+          <t>Civilization VI/Half-Life: Alyx/Stardew Valley</t>
         </is>
       </c>
       <c r="E2" s="2" t="n"/>
@@ -712,7 +712,7 @@
         </is>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="13.2" customHeight="1">
       <c r="A16" t="inlineStr">
         <is>
           <t>testnarek</t>
@@ -744,9 +744,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" ht="13.15" customHeight="1">
+    <row r="1" ht="13.2" customHeight="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>ID</t>
@@ -806,6 +806,11 @@
       <c r="F2" s="9" t="n">
         <v>2015</v>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1X2VR14/FA34HYR/I2YGGKN</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="5" t="n"/>
@@ -890,7 +895,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>AVDF58I/PFCG169</t>
+          <t>AVDF58I/PFCG169/3JU5UZG/J316TC4</t>
         </is>
       </c>
     </row>
@@ -917,6 +922,11 @@
       <c r="F6" s="9" t="n">
         <v>2016</v>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>NEI4N21/NHHSKM8</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="5" t="n"/>
@@ -943,7 +953,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Y6BAP56</t>
+          <t>P8EN5IW</t>
         </is>
       </c>
     </row>
@@ -1089,6 +1099,11 @@
       </c>
       <c r="F13" s="9" t="n">
         <v>2007</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>W4GAHQZ</t>
+        </is>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Fixed bug causing games to duplicate
</commit_message>
<xml_diff>
--- a/database_offline.xlsx
+++ b/database_offline.xlsx
@@ -409,10 +409,10 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="21.28515625" customWidth="1" min="3" max="3"/>
   </cols>
@@ -671,7 +671,7 @@
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>Civilization VI/Celeste/Half-Life: Alyx/The Witcher 3: Wild Hunt</t>
+          <t>Celeste/Half-Life: Alyx/The Witcher 3: Wild Hunt/Monkey Island/Prince of Persia/Command &amp; Conquer/Doom II: Hell on Earth/Age of Empires/The Sims/Quake/Counter-Strike/Team Fortress 2/Deus Ex/RollerCoaster Tycoon/Cuphead/Minecraft/Portal/Doom/Stardew Valley/Civilization VI</t>
         </is>
       </c>
     </row>
@@ -712,7 +712,7 @@
         </is>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="12.75" customHeight="1">
       <c r="A16" t="inlineStr">
         <is>
           <t>testnarek</t>

</xml_diff>

<commit_message>
added Friends and Friend Requests columns
</commit_message>
<xml_diff>
--- a/database_offline.xlsx
+++ b/database_offline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38610" yWindow="2550" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4950" yWindow="3225" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="accountInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -413,13 +413,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="21.28515625" customWidth="1" min="3" max="3"/>
   </cols>
@@ -445,6 +445,16 @@
           <t>Library/Civilization VI</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Friends</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Friend Requests</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -694,6 +704,11 @@
           <t>tommybones@yahoo.com</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Bob has sent you a friend request.&gt;&gt;Jose has sent you a friend request.</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
@@ -718,12 +733,17 @@
     <row r="16" ht="13.15" customHeight="1">
       <c r="A16" t="inlineStr">
         <is>
-          <t>testnarek</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Celeste/Half-Life: Alyx/Civilization VI/The Witcher 3: Wild Hunt/RollerCoaster Tycoon/Cuphead/Minecraft/Portal/Doom/Stardew Valley</t>
+          <t>Scooby</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>$coobyDoobyD00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>scoobysnacks@yahoo.com</t>
         </is>
       </c>
     </row>
@@ -747,7 +767,7 @@
       <selection activeCell="A2" sqref="A2:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="24.85546875" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>

</xml_diff>

<commit_message>
Fixed bug with games library not being updated after purchase
</commit_message>
<xml_diff>
--- a/database_offline.xlsx
+++ b/database_offline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4950" yWindow="3225" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38400" yWindow="2550" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="accountInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -68,13 +68,6 @@
       <color rgb="FF0D0D0D"/>
       <sz val="10"/>
     </font>
-    <font>
-      <name val="Arial"/>
-      <color theme="10"/>
-      <sz val="10"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -99,11 +92,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -121,10 +113,6 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -135,9 +123,8 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -408,7 +395,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
@@ -416,10 +403,10 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="21.28515625" customWidth="1" min="3" max="3"/>
   </cols>
@@ -686,7 +673,11 @@
           <t>nickb@gmail.com</t>
         </is>
       </c>
-      <c r="D13" s="3" t="n"/>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>The Witcher 3: Wild Hunt/Ori and the Blind Forest/Doom II: Hell on Earth</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
@@ -710,47 +701,46 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="inlineStr">
+    <row r="15" ht="13.15" customHeight="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Scooby</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>$coobyDoobyD00</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>scoobysnacks@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>narek98</t>
         </is>
       </c>
-      <c r="B15" s="12" t="n">
-        <v>123</v>
-      </c>
-      <c r="C15" s="11" t="inlineStr">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Welcome12345!</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>narek604@gmail.com</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Age of Empires/Rocket League/Civilization VI/Half-Life: Alyx/Celeste/Minecraft</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="13.15" customHeight="1">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Scooby</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>$coobyDoobyD00</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>scoobysnacks@yahoo.com</t>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>RollerCoaster Tycoon/Cuphead/Minecraft/Portal/Doom/Stardew Valley/Celeste/Half-Life: Alyx/Civilization VI/The Witcher 3: Wild Hunt/Team Fortress 2/Deus Ex/Counter-Strike/Quake</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -767,7 +757,7 @@
       <selection activeCell="A2" sqref="A2:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="24.85546875" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
@@ -826,7 +816,7 @@
           <t>CD Projekt Red</t>
         </is>
       </c>
-      <c r="D2" s="14" t="n">
+      <c r="D2" s="12" t="n">
         <v>29.99</v>
       </c>
       <c r="E2" s="9" t="inlineStr">
@@ -857,7 +847,7 @@
           <t>Firaxis Games</t>
         </is>
       </c>
-      <c r="D3" s="14" t="n">
+      <c r="D3" s="12" t="n">
         <v>59.99</v>
       </c>
       <c r="E3" s="9" t="inlineStr">
@@ -888,7 +878,7 @@
           <t>Valve Corporation</t>
         </is>
       </c>
-      <c r="D4" s="14" t="n">
+      <c r="D4" s="12" t="n">
         <v>59.99</v>
       </c>
       <c r="E4" s="9" t="inlineStr">
@@ -919,7 +909,7 @@
           <t>Matt Makes Games</t>
         </is>
       </c>
-      <c r="D5" s="14" t="n">
+      <c r="D5" s="12" t="n">
         <v>19.99</v>
       </c>
       <c r="E5" s="9" t="inlineStr">
@@ -950,7 +940,7 @@
           <t>ConcernedApe</t>
         </is>
       </c>
-      <c r="D6" s="14" t="n">
+      <c r="D6" s="12" t="n">
         <v>14.99</v>
       </c>
       <c r="E6" s="9" t="inlineStr">
@@ -981,7 +971,7 @@
           <t>id Software</t>
         </is>
       </c>
-      <c r="D7" s="14" t="n">
+      <c r="D7" s="12" t="n">
         <v>19.99</v>
       </c>
       <c r="E7" s="9" t="inlineStr">
@@ -1012,7 +1002,7 @@
           <t>Valve Corporation</t>
         </is>
       </c>
-      <c r="D8" s="14" t="n">
+      <c r="D8" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E8" s="9" t="inlineStr">
@@ -1038,7 +1028,7 @@
           <t>Mojang Studios</t>
         </is>
       </c>
-      <c r="D9" s="14" t="n">
+      <c r="D9" s="12" t="n">
         <v>26.95</v>
       </c>
       <c r="E9" s="9" t="inlineStr">
@@ -1064,7 +1054,7 @@
           <t>Studio MDHR</t>
         </is>
       </c>
-      <c r="D10" s="14" t="n">
+      <c r="D10" s="12" t="n">
         <v>19.99</v>
       </c>
       <c r="E10" s="9" t="inlineStr">
@@ -1090,7 +1080,7 @@
           <t>Chris Sawyer Productions</t>
         </is>
       </c>
-      <c r="D11" s="14" t="n">
+      <c r="D11" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E11" s="9" t="inlineStr">
@@ -1116,7 +1106,7 @@
           <t>Ion Storm</t>
         </is>
       </c>
-      <c r="D12" s="14" t="n">
+      <c r="D12" s="12" t="n">
         <v>6.99</v>
       </c>
       <c r="E12" s="9" t="inlineStr">
@@ -1142,7 +1132,7 @@
           <t>Valve Corporation</t>
         </is>
       </c>
-      <c r="D13" s="15" t="n">
+      <c r="D13" s="13" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="9" t="inlineStr">
@@ -1173,7 +1163,7 @@
           <t>Valve Corporation</t>
         </is>
       </c>
-      <c r="D14" s="14" t="n">
+      <c r="D14" s="12" t="n">
         <v>19.99</v>
       </c>
       <c r="E14" s="9" t="inlineStr">
@@ -1199,7 +1189,7 @@
           <t>id Software</t>
         </is>
       </c>
-      <c r="D15" s="14" t="n">
+      <c r="D15" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E15" s="9" t="inlineStr">
@@ -1225,7 +1215,7 @@
           <t>Maxis</t>
         </is>
       </c>
-      <c r="D16" s="14" t="n">
+      <c r="D16" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E16" s="9" t="inlineStr">
@@ -1251,7 +1241,7 @@
           <t>Ensemble Studios</t>
         </is>
       </c>
-      <c r="D17" s="14" t="n">
+      <c r="D17" s="12" t="n">
         <v>19.99</v>
       </c>
       <c r="E17" s="9" t="inlineStr">
@@ -1277,7 +1267,7 @@
           <t>id Software</t>
         </is>
       </c>
-      <c r="D18" s="14" t="n">
+      <c r="D18" s="12" t="n">
         <v>19.99</v>
       </c>
       <c r="E18" s="9" t="inlineStr">
@@ -1303,7 +1293,7 @@
           <t>Westwood Studios</t>
         </is>
       </c>
-      <c r="D19" s="14" t="n">
+      <c r="D19" s="12" t="n">
         <v>4.99</v>
       </c>
       <c r="E19" s="9" t="inlineStr">
@@ -1329,7 +1319,7 @@
           <t>Brøderbund</t>
         </is>
       </c>
-      <c r="D20" s="14" t="n">
+      <c r="D20" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E20" s="9" t="inlineStr">
@@ -1355,7 +1345,7 @@
           <t>LucasArts</t>
         </is>
       </c>
-      <c r="D21" s="14" t="n">
+      <c r="D21" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E21" s="9" t="inlineStr">
@@ -1381,7 +1371,7 @@
           <t>Cyan</t>
         </is>
       </c>
-      <c r="D22" s="14" t="n">
+      <c r="D22" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E22" s="9" t="inlineStr">
@@ -1407,7 +1397,7 @@
           <t>Chris Sawyer Productions</t>
         </is>
       </c>
-      <c r="D23" s="14" t="n">
+      <c r="D23" s="12" t="n">
         <v>5.99</v>
       </c>
       <c r="E23" s="9" t="inlineStr">
@@ -1433,7 +1423,7 @@
           <t>Interplay Entertainment</t>
         </is>
       </c>
-      <c r="D24" s="14" t="n">
+      <c r="D24" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E24" s="9" t="inlineStr">
@@ -1459,7 +1449,7 @@
           <t>Toby Fox</t>
         </is>
       </c>
-      <c r="D25" s="14" t="n">
+      <c r="D25" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E25" s="9" t="inlineStr">
@@ -1485,7 +1475,7 @@
           <t>ZA/UM</t>
         </is>
       </c>
-      <c r="D26" s="14" t="n">
+      <c r="D26" s="12" t="n">
         <v>9.99</v>
       </c>
       <c r="E26" s="9" t="inlineStr">
@@ -1511,7 +1501,7 @@
           <t>Yacht Club Games</t>
         </is>
       </c>
-      <c r="D27" s="14" t="n">
+      <c r="D27" s="12" t="n">
         <v>39.99</v>
       </c>
       <c r="E27" s="9" t="inlineStr">
@@ -1537,7 +1527,7 @@
           <t>Monstars Inc., Resonair</t>
         </is>
       </c>
-      <c r="D28" s="14" t="n">
+      <c r="D28" s="12" t="n">
         <v>24.99</v>
       </c>
       <c r="E28" s="9" t="inlineStr">
@@ -1563,7 +1553,7 @@
           <t>Supergiant Games</t>
         </is>
       </c>
-      <c r="D29" s="14" t="n">
+      <c r="D29" s="12" t="n">
         <v>39.99</v>
       </c>
       <c r="E29" s="9" t="inlineStr">
@@ -1589,7 +1579,7 @@
           <t>Moon Studios</t>
         </is>
       </c>
-      <c r="D30" s="14" t="n">
+      <c r="D30" s="12" t="n">
         <v>24.99</v>
       </c>
       <c r="E30" s="9" t="inlineStr">

</xml_diff>

<commit_message>
Added authorship, Fixed spacing in code
</commit_message>
<xml_diff>
--- a/database_offline.xlsx
+++ b/database_offline.xlsx
@@ -400,13 +400,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="21.28515625" customWidth="1" min="3" max="3"/>
   </cols>
@@ -737,6 +737,28 @@
       <c r="D16" t="inlineStr">
         <is>
           <t>RollerCoaster Tycoon/Cuphead/Minecraft/Portal/Doom/Stardew Valley/Celeste/Half-Life: Alyx/Civilization VI/The Witcher 3: Wild Hunt/Team Fortress 2/Deus Ex/Counter-Strike/Quake</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>random123</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Random1234!!</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>narek.asaturyan@gmail.com</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>The Witcher 3: Wild Hunt/Civilization VI/Half-Life: Alyx/Celeste/Stardew Valley/Doom</t>
         </is>
       </c>
     </row>
@@ -757,7 +779,7 @@
       <selection activeCell="A2" sqref="A2:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="24.85546875" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>

</xml_diff>